<commit_message>
re-structured so that when loaded from github the resources are located
</commit_message>
<xml_diff>
--- a/Book Flights/Default.xlsx
+++ b/Book Flights/Default.xlsx
@@ -1019,10 +1019,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyBorder="1" applyProtection="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
   </cellXfs>
@@ -2107,7 +2107,7 @@
       <c s="4" t="s">
         <v>205</v>
       </c>
-      <c s="7" t="s">
+      <c s="8" t="s">
         <v>74</v>
       </c>
       <c s="4" t="s">
@@ -2364,13 +2364,13 @@
       <c s="1"/>
       <c s="1"/>
       <c s="1"/>
-      <c s="8"/>
+      <c s="7"/>
     </row>
     <row s="2" customFormat="1">
       <c s="4" t="s">
         <v>0</v>
       </c>
-      <c s="7" t="s">
+      <c s="8" t="s">
         <v>205</v>
       </c>
       <c s="4"/>
@@ -2625,13 +2625,13 @@
       <c s="1"/>
       <c s="1"/>
       <c s="1"/>
-      <c s="8"/>
+      <c s="7"/>
     </row>
     <row s="2" customFormat="1">
       <c s="4" t="s">
         <v>244</v>
       </c>
-      <c s="7" t="s">
+      <c s="8" t="s">
         <v>89</v>
       </c>
       <c s="4"/>
@@ -2886,13 +2886,13 @@
       <c s="1"/>
       <c s="1"/>
       <c s="1"/>
-      <c s="8"/>
+      <c s="7"/>
     </row>
     <row s="2" customFormat="1">
       <c s="4" t="s">
         <v>89</v>
       </c>
-      <c s="7" t="s">
+      <c s="8" t="s">
         <v>244</v>
       </c>
       <c s="4"/>
@@ -3147,7 +3147,7 @@
       <c s="1"/>
       <c s="1"/>
       <c s="1"/>
-      <c s="8"/>
+      <c s="7"/>
     </row>
   </sheetData>
   <printOptions gridLines="1"/>

</xml_diff>

<commit_message>
corrected flights vs flight in odbc connection string
</commit_message>
<xml_diff>
--- a/Book Flights/Default.xlsx
+++ b/Book Flights/Default.xlsx
@@ -1013,10 +1013,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyBorder="1" applyProtection="1">
@@ -1330,9 +1330,9 @@
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="13.5"/>
   <cols>
     <col min="1" max="1" width="11.7109375" style="3" customWidth="1"/>
-    <col min="2" max="2" width="11.7109375" style="6" customWidth="1"/>
+    <col min="2" max="2" width="11.7109375" style="5" customWidth="1"/>
     <col min="3" max="3" width="11.7109375" style="3" customWidth="1"/>
-    <col min="4" max="255" width="9.140625" style="6" customWidth="1"/>
+    <col min="4" max="255" width="9.140625" style="5" customWidth="1"/>
     <col min="256" max="16384" width="9.140625" style="2" customWidth="1"/>
   </cols>
   <sheetData>
@@ -3240,10 +3240,10 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1484375" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="9.1484375" defaultRowHeight="13.5"/>
   <cols>
     <col min="1" max="1" width="14.5703125" style="3" customWidth="1"/>
-    <col min="2" max="2" width="230.140625" style="3" customWidth="1"/>
+    <col min="2" max="2" width="210.3203125" style="3" bestFit="1" customWidth="1"/>
     <col min="3" max="16384" width="9.1484375" style="2" customWidth="1"/>
   </cols>
   <sheetData>
@@ -3259,9 +3259,9 @@
       <c s="4" t="s">
         <v>45</v>
       </c>
-      <c s="5" t="str">
-        <f>"DSN=Flights;Database=C:\Users\"&amp;A2&amp;"\AppData\Local\UFT\Demo\DB\Flights.s3db;StepAPI=0;SyncPragma=;NoTXN=0;Timeout=;ShortNames=0;LongNames=0;NoCreat=0;NoWCHAR=0;FKSupport=0;JournalMode=;OEMCP=0;LoadExt=;BigInt=0;JDConv=0;PWD="</f>
-        <v>DSN=Flights;Database=C:\Users\someone\AppData\Local\UFT\Demo\DB\Flights.s3db;StepAPI=0;SyncPragma=;NoTXN=0;Timeout=;ShortNames=0;LongNames=0;NoCreat=0;NoWCHAR=0;FKSupport=0;JournalMode=;OEMCP=0;LoadExt=;BigInt=0;JDConv=0;PWD=</v>
+      <c s="6" t="str">
+        <f>"DSN=Flight;Database=C:\Users\"&amp;A2&amp;"\AppData\Local\UFT\Demo\DB\Flights.s3db;StepAPI=0;SyncPragma=;NoTXN=0;Timeout=;ShortNames=0;LongNames=0;NoCreat=0;NoWCHAR=0;FKSupport=0;JournalMode=;OEMCP=0;LoadExt=;BigInt=0;JDConv=0;PWD="</f>
+        <v>DSN=Flight;Database=C:\Users\someone\AppData\Local\UFT\Demo\DB\Flights.s3db;StepAPI=0;SyncPragma=;NoTXN=0;Timeout=;ShortNames=0;LongNames=0;NoCreat=0;NoWCHAR=0;FKSupport=0;JournalMode=;OEMCP=0;LoadExt=;BigInt=0;JDConv=0;PWD=</v>
       </c>
     </row>
   </sheetData>
@@ -3278,14 +3278,14 @@
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1484375" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="9.1484375" defaultRowHeight="13.5"/>
   <cols>
     <col min="1" max="1" width="14.5703125" style="2" customWidth="1"/>
-    <col min="2" max="2" width="224.28515625" style="3" customWidth="1"/>
+    <col min="2" max="2" width="209.3828125" style="3" bestFit="1" customWidth="1"/>
     <col min="3" max="16384" width="9.1484375" style="2" customWidth="1"/>
   </cols>
   <sheetData>
@@ -3301,63 +3301,63 @@
       <c s="1" t="s">
         <v>65</v>
       </c>
-      <c s="5" t="str">
-        <f t="shared" si="0" ref="B2:B8">"DSN=Flights;Database=C:\Users\"&amp;A2&amp;"\AppData\Local\UFT\Demo\DB\Flights.s3db;StepAPI=0;SyncPragma=;NoTXN=0;Timeout=;ShortNames=0;LongNames=0;NoCreat=0;NoWCHAR=0;FKSupport=0;JournalMode=;OEMCP=0;LoadExt=;BigInt=0;JDConv=0;PWD="</f>
-        <v>DSN=Flights;Database=C:\Users\somone\AppData\Local\UFT\Demo\DB\Flights.s3db;StepAPI=0;SyncPragma=;NoTXN=0;Timeout=;ShortNames=0;LongNames=0;NoCreat=0;NoWCHAR=0;FKSupport=0;JournalMode=;OEMCP=0;LoadExt=;BigInt=0;JDConv=0;PWD=</v>
+      <c s="6" t="str">
+        <f t="shared" si="0" ref="B2:B8">"DSN=Flight;Database=C:\Users\"&amp;A2&amp;"\AppData\Local\UFT\Demo\DB\Flights.s3db;StepAPI=0;SyncPragma=;NoTXN=0;Timeout=;ShortNames=0;LongNames=0;NoCreat=0;NoWCHAR=0;FKSupport=0;JournalMode=;OEMCP=0;LoadExt=;BigInt=0;JDConv=0;PWD="</f>
+        <v>DSN=Flight;Database=C:\Users\somone\AppData\Local\UFT\Demo\DB\Flights.s3db;StepAPI=0;SyncPragma=;NoTXN=0;Timeout=;ShortNames=0;LongNames=0;NoCreat=0;NoWCHAR=0;FKSupport=0;JournalMode=;OEMCP=0;LoadExt=;BigInt=0;JDConv=0;PWD=</v>
       </c>
     </row>
     <row s="2" customFormat="1">
       <c s="1" t="s">
         <v>65</v>
       </c>
-      <c s="5" t="str">
+      <c s="6" t="str">
         <f t="shared" si="0"/>
-        <v>DSN=Flights;Database=C:\Users\somone\AppData\Local\UFT\Demo\DB\Flights.s3db;StepAPI=0;SyncPragma=;NoTXN=0;Timeout=;ShortNames=0;LongNames=0;NoCreat=0;NoWCHAR=0;FKSupport=0;JournalMode=;OEMCP=0;LoadExt=;BigInt=0;JDConv=0;PWD=</v>
+        <v>DSN=Flight;Database=C:\Users\somone\AppData\Local\UFT\Demo\DB\Flights.s3db;StepAPI=0;SyncPragma=;NoTXN=0;Timeout=;ShortNames=0;LongNames=0;NoCreat=0;NoWCHAR=0;FKSupport=0;JournalMode=;OEMCP=0;LoadExt=;BigInt=0;JDConv=0;PWD=</v>
       </c>
     </row>
     <row s="2" customFormat="1">
       <c s="1" t="s">
         <v>65</v>
       </c>
-      <c s="5" t="str">
+      <c s="6" t="str">
         <f t="shared" si="0"/>
-        <v>DSN=Flights;Database=C:\Users\somone\AppData\Local\UFT\Demo\DB\Flights.s3db;StepAPI=0;SyncPragma=;NoTXN=0;Timeout=;ShortNames=0;LongNames=0;NoCreat=0;NoWCHAR=0;FKSupport=0;JournalMode=;OEMCP=0;LoadExt=;BigInt=0;JDConv=0;PWD=</v>
+        <v>DSN=Flight;Database=C:\Users\somone\AppData\Local\UFT\Demo\DB\Flights.s3db;StepAPI=0;SyncPragma=;NoTXN=0;Timeout=;ShortNames=0;LongNames=0;NoCreat=0;NoWCHAR=0;FKSupport=0;JournalMode=;OEMCP=0;LoadExt=;BigInt=0;JDConv=0;PWD=</v>
       </c>
     </row>
     <row ht="12.75" customHeight="1" s="2" customFormat="1">
       <c s="1" t="s">
         <v>65</v>
       </c>
-      <c s="5" t="str">
+      <c s="6" t="str">
         <f t="shared" si="0"/>
-        <v>DSN=Flights;Database=C:\Users\somone\AppData\Local\UFT\Demo\DB\Flights.s3db;StepAPI=0;SyncPragma=;NoTXN=0;Timeout=;ShortNames=0;LongNames=0;NoCreat=0;NoWCHAR=0;FKSupport=0;JournalMode=;OEMCP=0;LoadExt=;BigInt=0;JDConv=0;PWD=</v>
+        <v>DSN=Flight;Database=C:\Users\somone\AppData\Local\UFT\Demo\DB\Flights.s3db;StepAPI=0;SyncPragma=;NoTXN=0;Timeout=;ShortNames=0;LongNames=0;NoCreat=0;NoWCHAR=0;FKSupport=0;JournalMode=;OEMCP=0;LoadExt=;BigInt=0;JDConv=0;PWD=</v>
       </c>
     </row>
     <row s="2" customFormat="1">
       <c s="1" t="s">
         <v>65</v>
       </c>
-      <c s="5" t="str">
+      <c s="6" t="str">
         <f t="shared" si="0"/>
-        <v>DSN=Flights;Database=C:\Users\somone\AppData\Local\UFT\Demo\DB\Flights.s3db;StepAPI=0;SyncPragma=;NoTXN=0;Timeout=;ShortNames=0;LongNames=0;NoCreat=0;NoWCHAR=0;FKSupport=0;JournalMode=;OEMCP=0;LoadExt=;BigInt=0;JDConv=0;PWD=</v>
+        <v>DSN=Flight;Database=C:\Users\somone\AppData\Local\UFT\Demo\DB\Flights.s3db;StepAPI=0;SyncPragma=;NoTXN=0;Timeout=;ShortNames=0;LongNames=0;NoCreat=0;NoWCHAR=0;FKSupport=0;JournalMode=;OEMCP=0;LoadExt=;BigInt=0;JDConv=0;PWD=</v>
       </c>
     </row>
     <row s="2" customFormat="1">
       <c s="1" t="s">
         <v>65</v>
       </c>
-      <c s="5" t="str">
+      <c s="6" t="str">
         <f t="shared" si="0"/>
-        <v>DSN=Flights;Database=C:\Users\somone\AppData\Local\UFT\Demo\DB\Flights.s3db;StepAPI=0;SyncPragma=;NoTXN=0;Timeout=;ShortNames=0;LongNames=0;NoCreat=0;NoWCHAR=0;FKSupport=0;JournalMode=;OEMCP=0;LoadExt=;BigInt=0;JDConv=0;PWD=</v>
+        <v>DSN=Flight;Database=C:\Users\somone\AppData\Local\UFT\Demo\DB\Flights.s3db;StepAPI=0;SyncPragma=;NoTXN=0;Timeout=;ShortNames=0;LongNames=0;NoCreat=0;NoWCHAR=0;FKSupport=0;JournalMode=;OEMCP=0;LoadExt=;BigInt=0;JDConv=0;PWD=</v>
       </c>
     </row>
     <row s="2" customFormat="1">
       <c s="1" t="s">
         <v>65</v>
       </c>
-      <c s="5" t="str">
+      <c s="6" t="str">
         <f t="shared" si="0"/>
-        <v>DSN=Flights;Database=C:\Users\somone\AppData\Local\UFT\Demo\DB\Flights.s3db;StepAPI=0;SyncPragma=;NoTXN=0;Timeout=;ShortNames=0;LongNames=0;NoCreat=0;NoWCHAR=0;FKSupport=0;JournalMode=;OEMCP=0;LoadExt=;BigInt=0;JDConv=0;PWD=</v>
+        <v>DSN=Flight;Database=C:\Users\somone\AppData\Local\UFT\Demo\DB\Flights.s3db;StepAPI=0;SyncPragma=;NoTXN=0;Timeout=;ShortNames=0;LongNames=0;NoCreat=0;NoWCHAR=0;FKSupport=0;JournalMode=;OEMCP=0;LoadExt=;BigInt=0;JDConv=0;PWD=</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
changed Resuable to Reusable, and some other refactoring
</commit_message>
<xml_diff>
--- a/Book Flights/Default.xlsx
+++ b/Book Flights/Default.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="SpreadsheetGear 8.2.5.102"/>
   <workbookPr defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18075" windowHeight="9900" activeTab="5"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="18075" windowHeight="9900" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Global" sheetId="1" r:id="rId1"/>
@@ -13,6 +13,8 @@
     <sheet name="4 Select Flight" sheetId="4" r:id="rId4"/>
     <sheet name="5 Flight Confirmation" sheetId="5" r:id="rId5"/>
     <sheet name="6 Search Order" sheetId="6" r:id="rId6"/>
+    <sheet name="1 Open Application {Reusable}" sheetId="7" r:id="rId7"/>
+    <sheet name="7 Close Application {Reusable}" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="40001"/>
 </workbook>
@@ -1010,22 +1012,22 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
   </cellXfs>
@@ -1332,10 +1334,10 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="13.5"/>
   <cols>
-    <col min="1" max="1" width="11.7109375" style="4" customWidth="1"/>
-    <col min="2" max="2" width="11.7109375" style="6" customWidth="1"/>
-    <col min="3" max="3" width="11.7109375" style="4" customWidth="1"/>
-    <col min="4" max="255" width="9.140625" style="6" customWidth="1"/>
+    <col min="1" max="1" width="11.7109375" style="3" customWidth="1"/>
+    <col min="2" max="2" width="11.7109375" style="5" customWidth="1"/>
+    <col min="3" max="3" width="11.7109375" style="3" customWidth="1"/>
+    <col min="4" max="255" width="9.140625" style="5" customWidth="1"/>
     <col min="256" max="16384" width="9.140625" style="2" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2107,13 +2109,13 @@
       </c>
     </row>
     <row s="2" customFormat="1">
-      <c s="3" t="s">
+      <c s="4" t="s">
         <v>206</v>
       </c>
-      <c s="7" t="s">
+      <c s="8" t="s">
         <v>75</v>
       </c>
-      <c s="3" t="s">
+      <c s="4" t="s">
         <v>1</v>
       </c>
       <c s="1"/>
@@ -2367,790 +2369,790 @@
       <c s="1"/>
       <c s="1"/>
       <c s="1"/>
-      <c s="5"/>
+      <c s="6"/>
     </row>
     <row s="2" customFormat="1">
-      <c s="3" t="s">
+      <c s="4" t="s">
         <v>0</v>
       </c>
-      <c s="7" t="s">
+      <c s="8" t="s">
         <v>206</v>
       </c>
-      <c s="3"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="5"/>
+      <c s="4"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="6"/>
     </row>
     <row s="2" customFormat="1">
-      <c s="3" t="s">
+      <c s="4" t="s">
         <v>245</v>
       </c>
-      <c s="7" t="s">
+      <c s="8" t="s">
         <v>90</v>
       </c>
-      <c s="3"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="5"/>
+      <c s="4"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="6"/>
     </row>
     <row s="2" customFormat="1">
-      <c s="3" t="s">
+      <c s="4" t="s">
         <v>90</v>
       </c>
-      <c s="7" t="s">
+      <c s="8" t="s">
         <v>245</v>
       </c>
-      <c s="3"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="5"/>
+      <c s="4"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="6"/>
     </row>
   </sheetData>
   <printOptions gridLines="1"/>
@@ -3245,8 +3247,8 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1484375" defaultRowHeight="13.5"/>
   <cols>
-    <col min="1" max="1" width="14.5703125" style="4" customWidth="1"/>
-    <col min="2" max="2" width="211.078125" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.5703125" style="3" customWidth="1"/>
+    <col min="2" max="2" width="211.078125" style="3" bestFit="1" customWidth="1"/>
     <col min="3" max="16384" width="9.1484375" style="2" customWidth="1"/>
   </cols>
   <sheetData>
@@ -3259,10 +3261,10 @@
       </c>
     </row>
     <row s="2" customFormat="1">
-      <c s="3" t="s">
+      <c s="4" t="s">
         <v>45</v>
       </c>
-      <c s="8" t="str">
+      <c s="7" t="str">
         <f>"DSN=Flights;Database=C:\Users\"&amp;A2&amp;"\AppData\Local\UFT\Demo\DB\Flights.s3db;StepAPI=0;SyncPragma=;NoTXN=0;Timeout=;ShortNames=0;LongNames=0;NoCreat=0;NoWCHAR=0;FKSupport=0;JournalMode=;OEMCP=0;LoadExt=;BigInt=0;JDConv=0;PWD="</f>
         <v>DSN=Flights;Database=C:\Users\someone\AppData\Local\UFT\Demo\DB\Flights.s3db;StepAPI=0;SyncPragma=;NoTXN=0;Timeout=;ShortNames=0;LongNames=0;NoCreat=0;NoWCHAR=0;FKSupport=0;JournalMode=;OEMCP=0;LoadExt=;BigInt=0;JDConv=0;PWD=</v>
       </c>
@@ -3281,14 +3283,14 @@
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1484375" defaultRowHeight="13.5"/>
   <cols>
     <col min="1" max="1" width="12.109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="210.140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="210.140625" style="3" bestFit="1" customWidth="1"/>
     <col min="3" max="5" width="9.41796875" style="2" customWidth="1"/>
     <col min="6" max="16384" width="9.1484375" style="2" customWidth="1"/>
   </cols>
@@ -3314,85 +3316,85 @@
       <c s="1" t="s">
         <v>65</v>
       </c>
-      <c s="3" t="str">
+      <c s="4" t="str">
         <f t="shared" si="0" ref="B2:B8">"DSN=Flights;Database=C:\Users\"&amp;A2&amp;"\AppData\Local\UFT\Demo\DB\Flights.s3db;StepAPI=0;SyncPragma=;NoTXN=0;Timeout=;ShortNames=0;LongNames=0;NoCreat=0;NoWCHAR=0;FKSupport=0;JournalMode=;OEMCP=0;LoadExt=;BigInt=0;JDConv=0;PWD="</f>
         <v>DSN=Flights;Database=C:\Users\somone\AppData\Local\UFT\Demo\DB\Flights.s3db;StepAPI=0;SyncPragma=;NoTXN=0;Timeout=;ShortNames=0;LongNames=0;NoCreat=0;NoWCHAR=0;FKSupport=0;JournalMode=;OEMCP=0;LoadExt=;BigInt=0;JDConv=0;PWD=</v>
       </c>
       <c s="1"/>
       <c s="1"/>
-      <c s="5"/>
+      <c s="6"/>
     </row>
     <row s="2" customFormat="1">
       <c s="1" t="s">
         <v>65</v>
       </c>
-      <c s="3" t="str">
+      <c s="4" t="str">
         <f t="shared" si="0"/>
         <v>DSN=Flights;Database=C:\Users\somone\AppData\Local\UFT\Demo\DB\Flights.s3db;StepAPI=0;SyncPragma=;NoTXN=0;Timeout=;ShortNames=0;LongNames=0;NoCreat=0;NoWCHAR=0;FKSupport=0;JournalMode=;OEMCP=0;LoadExt=;BigInt=0;JDConv=0;PWD=</v>
       </c>
       <c s="1"/>
       <c s="1"/>
-      <c s="5"/>
+      <c s="6"/>
     </row>
     <row s="2" customFormat="1">
       <c s="1" t="s">
         <v>65</v>
       </c>
-      <c s="3" t="str">
+      <c s="4" t="str">
         <f t="shared" si="0"/>
         <v>DSN=Flights;Database=C:\Users\somone\AppData\Local\UFT\Demo\DB\Flights.s3db;StepAPI=0;SyncPragma=;NoTXN=0;Timeout=;ShortNames=0;LongNames=0;NoCreat=0;NoWCHAR=0;FKSupport=0;JournalMode=;OEMCP=0;LoadExt=;BigInt=0;JDConv=0;PWD=</v>
       </c>
       <c s="1"/>
       <c s="1"/>
-      <c s="5"/>
+      <c s="6"/>
     </row>
     <row ht="12.75" customHeight="1" s="2" customFormat="1">
       <c s="1" t="s">
         <v>65</v>
       </c>
-      <c s="3" t="str">
+      <c s="4" t="str">
         <f t="shared" si="0"/>
         <v>DSN=Flights;Database=C:\Users\somone\AppData\Local\UFT\Demo\DB\Flights.s3db;StepAPI=0;SyncPragma=;NoTXN=0;Timeout=;ShortNames=0;LongNames=0;NoCreat=0;NoWCHAR=0;FKSupport=0;JournalMode=;OEMCP=0;LoadExt=;BigInt=0;JDConv=0;PWD=</v>
       </c>
       <c s="1"/>
       <c s="1"/>
-      <c s="5"/>
+      <c s="6"/>
     </row>
     <row s="2" customFormat="1">
       <c s="1" t="s">
         <v>65</v>
       </c>
-      <c s="3" t="str">
+      <c s="4" t="str">
         <f t="shared" si="0"/>
         <v>DSN=Flights;Database=C:\Users\somone\AppData\Local\UFT\Demo\DB\Flights.s3db;StepAPI=0;SyncPragma=;NoTXN=0;Timeout=;ShortNames=0;LongNames=0;NoCreat=0;NoWCHAR=0;FKSupport=0;JournalMode=;OEMCP=0;LoadExt=;BigInt=0;JDConv=0;PWD=</v>
       </c>
       <c s="1"/>
       <c s="1"/>
-      <c s="5"/>
+      <c s="6"/>
     </row>
     <row s="2" customFormat="1">
       <c s="1" t="s">
         <v>65</v>
       </c>
-      <c s="3" t="str">
+      <c s="4" t="str">
         <f t="shared" si="0"/>
         <v>DSN=Flights;Database=C:\Users\somone\AppData\Local\UFT\Demo\DB\Flights.s3db;StepAPI=0;SyncPragma=;NoTXN=0;Timeout=;ShortNames=0;LongNames=0;NoCreat=0;NoWCHAR=0;FKSupport=0;JournalMode=;OEMCP=0;LoadExt=;BigInt=0;JDConv=0;PWD=</v>
       </c>
       <c s="1"/>
       <c s="1"/>
-      <c s="5"/>
+      <c s="6"/>
     </row>
     <row s="2" customFormat="1">
       <c s="1" t="s">
         <v>65</v>
       </c>
-      <c s="3" t="str">
+      <c s="4" t="str">
         <f t="shared" si="0"/>
         <v>DSN=Flights;Database=C:\Users\somone\AppData\Local\UFT\Demo\DB\Flights.s3db;StepAPI=0;SyncPragma=;NoTXN=0;Timeout=;ShortNames=0;LongNames=0;NoCreat=0;NoWCHAR=0;FKSupport=0;JournalMode=;OEMCP=0;LoadExt=;BigInt=0;JDConv=0;PWD=</v>
       </c>
       <c s="1"/>
       <c s="1"/>
-      <c s="5"/>
+      <c s="6"/>
     </row>
   </sheetData>
   <printOptions gridLines="1"/>
@@ -3402,4 +3404,42 @@
     <oddFooter>&amp;CPage &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75"/>
+  <cols>
+    <col min="1" max="16384" width="9.078125" style="2" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row ht="12.75" customHeight="1" customFormat="1"/>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75"/>
+  <cols>
+    <col min="1" max="16384" width="9.078125" style="2" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row ht="12.75" customHeight="1" customFormat="1"/>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
moved Reusable test within the Book Flights test, so that it is found without modifying the Settings->Directory value
</commit_message>
<xml_diff>
--- a/Book Flights/Default.xlsx
+++ b/Book Flights/Default.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="SpreadsheetGear 8.2.5.102"/>
   <workbookPr defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18075" windowHeight="9900" activeTab="7"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="18075" windowHeight="9900" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="Global" sheetId="1" r:id="rId1"/>
@@ -15,6 +15,7 @@
     <sheet name="6 Search Order" sheetId="6" r:id="rId6"/>
     <sheet name="1 Open Application {Reusable}" sheetId="7" r:id="rId7"/>
     <sheet name="7 Close Application {Reusable}" sheetId="8" r:id="rId8"/>
+    <sheet name="Sheet9" sheetId="9" r:id="rId9"/>
   </sheets>
   <calcPr calcId="40001"/>
 </workbook>
@@ -1004,7 +1005,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
@@ -1012,10 +1013,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
@@ -1028,6 +1029,9 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
   </cellXfs>
@@ -1334,9 +1338,9 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="13.5"/>
   <cols>
-    <col min="1" max="1" width="11.7109375" style="3" customWidth="1"/>
+    <col min="1" max="1" width="11.7109375" style="4" customWidth="1"/>
     <col min="2" max="2" width="11.7109375" style="5" customWidth="1"/>
-    <col min="3" max="3" width="11.7109375" style="3" customWidth="1"/>
+    <col min="3" max="3" width="11.7109375" style="4" customWidth="1"/>
     <col min="4" max="255" width="9.140625" style="5" customWidth="1"/>
     <col min="256" max="16384" width="9.140625" style="2" customWidth="1"/>
   </cols>
@@ -2109,13 +2113,13 @@
       </c>
     </row>
     <row s="2" customFormat="1">
-      <c s="4" t="s">
+      <c s="3" t="s">
         <v>206</v>
       </c>
       <c s="8" t="s">
         <v>75</v>
       </c>
-      <c s="4" t="s">
+      <c s="3" t="s">
         <v>1</v>
       </c>
       <c s="1"/>
@@ -2372,13 +2376,13 @@
       <c s="6"/>
     </row>
     <row s="2" customFormat="1">
-      <c s="4" t="s">
+      <c s="3" t="s">
         <v>0</v>
       </c>
       <c s="8" t="s">
         <v>206</v>
       </c>
-      <c s="4"/>
+      <c s="3"/>
       <c s="1"/>
       <c s="1"/>
       <c s="1"/>
@@ -2633,13 +2637,13 @@
       <c s="6"/>
     </row>
     <row s="2" customFormat="1">
-      <c s="4" t="s">
+      <c s="3" t="s">
         <v>245</v>
       </c>
       <c s="8" t="s">
         <v>90</v>
       </c>
-      <c s="4"/>
+      <c s="3"/>
       <c s="1"/>
       <c s="1"/>
       <c s="1"/>
@@ -2894,13 +2898,13 @@
       <c s="6"/>
     </row>
     <row s="2" customFormat="1">
-      <c s="4" t="s">
+      <c s="3" t="s">
         <v>90</v>
       </c>
       <c s="8" t="s">
         <v>245</v>
       </c>
-      <c s="4"/>
+      <c s="3"/>
       <c s="1"/>
       <c s="1"/>
       <c s="1"/>
@@ -3247,8 +3251,8 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1484375" defaultRowHeight="13.5"/>
   <cols>
-    <col min="1" max="1" width="14.5703125" style="3" customWidth="1"/>
-    <col min="2" max="2" width="211.078125" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.5703125" style="4" customWidth="1"/>
+    <col min="2" max="2" width="211.078125" style="4" bestFit="1" customWidth="1"/>
     <col min="3" max="16384" width="9.1484375" style="2" customWidth="1"/>
   </cols>
   <sheetData>
@@ -3261,7 +3265,7 @@
       </c>
     </row>
     <row s="2" customFormat="1">
-      <c s="4" t="s">
+      <c s="3" t="s">
         <v>45</v>
       </c>
       <c s="7" t="str">
@@ -3290,7 +3294,7 @@
   <sheetFormatPr defaultColWidth="9.1484375" defaultRowHeight="13.5"/>
   <cols>
     <col min="1" max="1" width="12.109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="210.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="210.140625" style="4" bestFit="1" customWidth="1"/>
     <col min="3" max="5" width="9.41796875" style="2" customWidth="1"/>
     <col min="6" max="16384" width="9.1484375" style="2" customWidth="1"/>
   </cols>
@@ -3316,7 +3320,7 @@
       <c s="1" t="s">
         <v>65</v>
       </c>
-      <c s="4" t="str">
+      <c s="3" t="str">
         <f t="shared" si="0" ref="B2:B8">"DSN=Flights;Database=C:\Users\"&amp;A2&amp;"\AppData\Local\UFT\Demo\DB\Flights.s3db;StepAPI=0;SyncPragma=;NoTXN=0;Timeout=;ShortNames=0;LongNames=0;NoCreat=0;NoWCHAR=0;FKSupport=0;JournalMode=;OEMCP=0;LoadExt=;BigInt=0;JDConv=0;PWD="</f>
         <v>DSN=Flights;Database=C:\Users\somone\AppData\Local\UFT\Demo\DB\Flights.s3db;StepAPI=0;SyncPragma=;NoTXN=0;Timeout=;ShortNames=0;LongNames=0;NoCreat=0;NoWCHAR=0;FKSupport=0;JournalMode=;OEMCP=0;LoadExt=;BigInt=0;JDConv=0;PWD=</v>
       </c>
@@ -3328,7 +3332,7 @@
       <c s="1" t="s">
         <v>65</v>
       </c>
-      <c s="4" t="str">
+      <c s="3" t="str">
         <f t="shared" si="0"/>
         <v>DSN=Flights;Database=C:\Users\somone\AppData\Local\UFT\Demo\DB\Flights.s3db;StepAPI=0;SyncPragma=;NoTXN=0;Timeout=;ShortNames=0;LongNames=0;NoCreat=0;NoWCHAR=0;FKSupport=0;JournalMode=;OEMCP=0;LoadExt=;BigInt=0;JDConv=0;PWD=</v>
       </c>
@@ -3340,7 +3344,7 @@
       <c s="1" t="s">
         <v>65</v>
       </c>
-      <c s="4" t="str">
+      <c s="3" t="str">
         <f t="shared" si="0"/>
         <v>DSN=Flights;Database=C:\Users\somone\AppData\Local\UFT\Demo\DB\Flights.s3db;StepAPI=0;SyncPragma=;NoTXN=0;Timeout=;ShortNames=0;LongNames=0;NoCreat=0;NoWCHAR=0;FKSupport=0;JournalMode=;OEMCP=0;LoadExt=;BigInt=0;JDConv=0;PWD=</v>
       </c>
@@ -3352,7 +3356,7 @@
       <c s="1" t="s">
         <v>65</v>
       </c>
-      <c s="4" t="str">
+      <c s="3" t="str">
         <f t="shared" si="0"/>
         <v>DSN=Flights;Database=C:\Users\somone\AppData\Local\UFT\Demo\DB\Flights.s3db;StepAPI=0;SyncPragma=;NoTXN=0;Timeout=;ShortNames=0;LongNames=0;NoCreat=0;NoWCHAR=0;FKSupport=0;JournalMode=;OEMCP=0;LoadExt=;BigInt=0;JDConv=0;PWD=</v>
       </c>
@@ -3364,7 +3368,7 @@
       <c s="1" t="s">
         <v>65</v>
       </c>
-      <c s="4" t="str">
+      <c s="3" t="str">
         <f t="shared" si="0"/>
         <v>DSN=Flights;Database=C:\Users\somone\AppData\Local\UFT\Demo\DB\Flights.s3db;StepAPI=0;SyncPragma=;NoTXN=0;Timeout=;ShortNames=0;LongNames=0;NoCreat=0;NoWCHAR=0;FKSupport=0;JournalMode=;OEMCP=0;LoadExt=;BigInt=0;JDConv=0;PWD=</v>
       </c>
@@ -3376,7 +3380,7 @@
       <c s="1" t="s">
         <v>65</v>
       </c>
-      <c s="4" t="str">
+      <c s="3" t="str">
         <f t="shared" si="0"/>
         <v>DSN=Flights;Database=C:\Users\somone\AppData\Local\UFT\Demo\DB\Flights.s3db;StepAPI=0;SyncPragma=;NoTXN=0;Timeout=;ShortNames=0;LongNames=0;NoCreat=0;NoWCHAR=0;FKSupport=0;JournalMode=;OEMCP=0;LoadExt=;BigInt=0;JDConv=0;PWD=</v>
       </c>
@@ -3388,7 +3392,7 @@
       <c s="1" t="s">
         <v>65</v>
       </c>
-      <c s="4" t="str">
+      <c s="3" t="str">
         <f t="shared" si="0"/>
         <v>DSN=Flights;Database=C:\Users\somone\AppData\Local\UFT\Demo\DB\Flights.s3db;StepAPI=0;SyncPragma=;NoTXN=0;Timeout=;ShortNames=0;LongNames=0;NoCreat=0;NoWCHAR=0;FKSupport=0;JournalMode=;OEMCP=0;LoadExt=;BigInt=0;JDConv=0;PWD=</v>
       </c>
@@ -3429,7 +3433,7 @@
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -3442,4 +3446,23 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.1"/>
+  <cols>
+    <col min="1" max="16384" width="9.078125" style="9" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row customFormat="1"/>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
changed the location of the Reusable test
</commit_message>
<xml_diff>
--- a/Book Flights/Default.xlsx
+++ b/Book Flights/Default.xlsx
@@ -1017,16 +1017,16 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
@@ -1337,9 +1337,9 @@
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="13.5"/>
   <cols>
     <col min="1" max="1" width="11.7109375" style="3" customWidth="1"/>
-    <col min="2" max="2" width="11.7109375" style="6" customWidth="1"/>
+    <col min="2" max="2" width="11.7109375" style="5" customWidth="1"/>
     <col min="3" max="3" width="11.7109375" style="3" customWidth="1"/>
-    <col min="4" max="255" width="9.140625" style="6" customWidth="1"/>
+    <col min="4" max="255" width="9.140625" style="5" customWidth="1"/>
     <col min="256" max="16384" width="9.140625" style="2" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2371,7 +2371,7 @@
       <c r="IR2" s="1"/>
       <c r="IS2" s="1"/>
       <c r="IT2" s="1"/>
-      <c r="IU2" s="5"/>
+      <c r="IU2" s="6"/>
     </row>
     <row r="3" s="2" customFormat="1">
       <c r="A3" s="4" t="s">
@@ -2632,7 +2632,7 @@
       <c r="IR3" s="1"/>
       <c r="IS3" s="1"/>
       <c r="IT3" s="1"/>
-      <c r="IU3" s="5"/>
+      <c r="IU3" s="6"/>
     </row>
     <row r="4" s="2" customFormat="1">
       <c r="A4" s="4" t="s">
@@ -2893,7 +2893,7 @@
       <c r="IR4" s="1"/>
       <c r="IS4" s="1"/>
       <c r="IT4" s="1"/>
-      <c r="IU4" s="5"/>
+      <c r="IU4" s="6"/>
     </row>
     <row r="5" s="2" customFormat="1">
       <c r="A5" s="4" t="s">
@@ -3154,7 +3154,7 @@
       <c r="IR5" s="1"/>
       <c r="IS5" s="1"/>
       <c r="IT5" s="1"/>
-      <c r="IU5" s="5"/>
+      <c r="IU5" s="6"/>
     </row>
   </sheetData>
   <printOptions gridLines="1"/>
@@ -3266,7 +3266,7 @@
       <c r="A2" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="B2" s="8" t="str">
+      <c r="B2" s="7" t="str">
         <f>"DSN=Flights;Database=C:\Users\"&amp;A2&amp;"\AppData\Local\UFT\Demo\DB\Flights.s3db;StepAPI=0;SyncPragma=;NoTXN=0;Timeout=;ShortNames=0;LongNames=0;NoCreat=0;NoWCHAR=0;FKSupport=0;JournalMode=;OEMCP=0;LoadExt=;BigInt=0;JDConv=0;PWD="</f>
         <v>DSN=Flights;Database=C:\Users\someone\AppData\Local\UFT\Demo\DB\Flights.s3db;StepAPI=0;SyncPragma=;NoTXN=0;Timeout=;ShortNames=0;LongNames=0;NoCreat=0;NoWCHAR=0;FKSupport=0;JournalMode=;OEMCP=0;LoadExt=;BigInt=0;JDConv=0;PWD=</v>
       </c>
@@ -3324,7 +3324,7 @@
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
-      <c r="E2" s="5"/>
+      <c r="E2" s="6"/>
     </row>
     <row r="3" s="2" customFormat="1">
       <c r="A3" s="1" t="s">
@@ -3336,7 +3336,7 @@
       </c>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
-      <c r="E3" s="5"/>
+      <c r="E3" s="6"/>
     </row>
     <row r="4" s="2" customFormat="1">
       <c r="A4" s="1" t="s">
@@ -3348,7 +3348,7 @@
       </c>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
-      <c r="E4" s="5"/>
+      <c r="E4" s="6"/>
     </row>
     <row r="5" ht="12.75" customHeight="1" s="2" customFormat="1">
       <c r="A5" s="1" t="s">
@@ -3360,7 +3360,7 @@
       </c>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
-      <c r="E5" s="5"/>
+      <c r="E5" s="6"/>
     </row>
     <row r="6" s="2" customFormat="1">
       <c r="A6" s="1" t="s">
@@ -3372,7 +3372,7 @@
       </c>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
-      <c r="E6" s="5"/>
+      <c r="E6" s="6"/>
     </row>
     <row r="7" s="2" customFormat="1">
       <c r="A7" s="1" t="s">
@@ -3384,7 +3384,7 @@
       </c>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
-      <c r="E7" s="5"/>
+      <c r="E7" s="6"/>
     </row>
     <row r="8" s="2" customFormat="1">
       <c r="A8" s="1" t="s">
@@ -3396,7 +3396,7 @@
       </c>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
-      <c r="E8" s="5"/>
+      <c r="E8" s="6"/>
     </row>
   </sheetData>
   <printOptions gridLines="1"/>
@@ -3418,7 +3418,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.1"/>
   <cols>
-    <col min="1" max="16384" width="9.078125" style="7" customWidth="1"/>
+    <col min="1" max="16384" width="9.078125" style="8" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="1"/>

</xml_diff>